<commit_message>
Made effect times calculator spreadsheet prettier
</commit_message>
<xml_diff>
--- a/effect_times_calculator.xlsx
+++ b/effect_times_calculator.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>values</t>
   </si>
   <si>
     <t>offset 1</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>offset 2</t>
@@ -81,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +89,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -128,6 +131,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -215,13 +225,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -273,73 +276,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -655,57 +661,57 @@
     <col min="1" max="1" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="21" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="21" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="23" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="23" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="23" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="23" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="24" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="24" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="24" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -713,128 +719,126 @@
         <v>1</v>
       </c>
       <c r="E3" s="5"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="D5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
+      <c r="D6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="11">
         <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="12">
         <f>ROUNDUP($E$3/$C9,0)*$C9</f>
@@ -870,12 +874,12 @@
         <f>N9+$C9</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="7" t="s">
-        <v>12</v>
+      <c r="D10" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="15">
         <f>ROUNDUP($E$4/$C9,0)*$C9</f>
@@ -911,12 +915,12 @@
         <f>N10+$C9</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
+      <c r="D11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="15">
         <f>ROUNDUP($E$5/$C9,0)*$C9</f>
@@ -956,8 +960,8 @@
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="9" t="s">
-        <v>14</v>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E12" s="15">
         <f>ROUNDUP($E$6/$C9,0)*$C9</f>
@@ -993,16 +997,16 @@
         <f>N12+$C9</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="11">
         <v>45</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="12">
         <f>ROUNDUP($E$3/$C13,0)*$C13</f>
@@ -1038,12 +1042,12 @@
         <f>N13+$C13</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="7" t="s">
-        <v>12</v>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E14" s="15">
         <f>ROUNDUP($E$4/$C13,0)*$C13</f>
@@ -1079,12 +1083,12 @@
         <f>N14+$C13</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="7" t="s">
-        <v>13</v>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E15" s="15">
         <f>ROUNDUP($E$5/$C13,0)*$C13</f>
@@ -1124,8 +1128,8 @@
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="9" t="s">
-        <v>14</v>
+      <c r="D16" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E16" s="15">
         <f>ROUNDUP($E$6/$C13,0)*$C13</f>
@@ -1161,16 +1165,16 @@
         <f>N16+$C13</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="11">
         <f>60+40</f>
       </c>
       <c r="D17" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="12">
         <f>ROUNDUP($E$3/$C17,0)*$C17</f>
@@ -1206,12 +1210,12 @@
         <f>N17+$C17</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
+      <c r="D18" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E18" s="15">
         <f>ROUNDUP($E$4/$C17,0)*$C17</f>
@@ -1247,12 +1251,12 @@
         <f>N18+$C17</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="7" t="s">
-        <v>13</v>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E19" s="15">
         <f>ROUNDUP($E$5/$C17,0)*$C17</f>
@@ -1292,8 +1296,8 @@
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="9" t="s">
-        <v>14</v>
+      <c r="D20" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E20" s="15">
         <f>ROUNDUP($E$6/$C17,0)*$C17</f>
@@ -1329,16 +1333,16 @@
         <f>N20+$C17</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="11">
         <f>60*2</f>
       </c>
       <c r="D21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="12">
         <f>ROUNDUP($E$3/$C21,0)*$C21</f>
@@ -1374,12 +1378,12 @@
         <f>N21+$C21</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="7" t="s">
-        <v>12</v>
+      <c r="D22" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E22" s="15">
         <f>ROUNDUP($E$4/$C21,0)*$C21</f>
@@ -1415,12 +1419,12 @@
         <f>N22+$C21</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="7" t="s">
-        <v>13</v>
+      <c r="D23" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="15">
         <f>ROUNDUP($E$5/$C21,0)*$C21</f>
@@ -1460,8 +1464,8 @@
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="9" t="s">
-        <v>14</v>
+      <c r="D24" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E24" s="15">
         <f>ROUNDUP($E$6/$C21,0)*$C21</f>
@@ -1497,16 +1501,16 @@
         <f>N24+$C21</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="11">
         <f>60*3</f>
       </c>
       <c r="D25" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="12">
         <f>ROUNDUP($E$3/$C25,0)*$C25</f>
@@ -1542,12 +1546,12 @@
         <f>N25+$C25</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="7" t="s">
-        <v>12</v>
+      <c r="D26" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E26" s="15">
         <f>ROUNDUP($E$4/$C25,0)*$C25</f>
@@ -1583,12 +1587,12 @@
         <f>N26+$C25</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="7" t="s">
-        <v>13</v>
+      <c r="D27" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E27" s="15">
         <f>ROUNDUP($E$5/$C25,0)*$C25</f>
@@ -1628,8 +1632,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="9" t="s">
-        <v>14</v>
+      <c r="D28" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E28" s="15">
         <f>ROUNDUP($E$6/$C25,0)*$C25</f>
@@ -1665,16 +1669,16 @@
         <f>N28+$C25</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="11">
         <f>60*5</f>
       </c>
       <c r="D29" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E29" s="12">
         <f>ROUNDUP($E$3/$C29,0)*$C29</f>
@@ -1710,12 +1714,12 @@
         <f>N29+$C29</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="7" t="s">
-        <v>12</v>
+      <c r="D30" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E30" s="15">
         <f>ROUNDUP($E$4/$C29,0)*$C29</f>
@@ -1751,12 +1755,12 @@
         <f>N30+$C29</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="7" t="s">
-        <v>13</v>
+      <c r="D31" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E31" s="15">
         <f>ROUNDUP($E$5/$C29,0)*$C29</f>
@@ -1792,12 +1796,12 @@
         <f>N31+$C29</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="9" t="s">
-        <v>14</v>
+      <c r="D32" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="E32" s="18">
         <f>ROUNDUP($E$6/$C29,0)*$C29</f>

</xml_diff>